<commit_message>
add struct _s names like quake to all structs
</commit_message>
<xml_diff>
--- a/Design/Euphoria Rev1 Task List.xlsx
+++ b/Design/Euphoria Rev1 Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Euphoria\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86B93641-6CA9-4F54-8F2C-1D48C1728B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30EA8ED-FA61-4EC3-968D-9A2DC5DFFCF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11895" yWindow="1815" windowWidth="21615" windowHeight="11325" activeTab="3" xr2:uid="{283B4835-3097-4296-82F0-26B49D49393F}"/>
+    <workbookView xWindow="12435" yWindow="750" windowWidth="21615" windowHeight="11325" activeTab="3" xr2:uid="{283B4835-3097-4296-82F0-26B49D49393F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tier 0" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>Euphoria</t>
   </si>
@@ -141,6 +141,42 @@
   </si>
   <si>
     <t>Tier 3 Feature List</t>
+  </si>
+  <si>
+    <t>Tier 4 Feature List</t>
+  </si>
+  <si>
+    <t>Last Updated: July 19, 2023</t>
+  </si>
+  <si>
+    <t>Null Renderer</t>
+  </si>
+  <si>
+    <t>OpenGL Renderer</t>
+  </si>
+  <si>
+    <t>SDL2 Renderer</t>
+  </si>
+  <si>
+    <t>Tasks:</t>
+  </si>
+  <si>
+    <t>GameObject</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>GameObject: Squirrel Exposure</t>
+  </si>
+  <si>
+    <t>Euphoria Post-Tier4</t>
+  </si>
+  <si>
+    <t>Object Properties</t>
+  </si>
+  <si>
+    <t>Objects:</t>
   </si>
 </sst>
 </file>
@@ -195,12 +231,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -519,7 +554,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A16:A17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -556,7 +591,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -572,7 +607,7 @@
       <c r="D5" s="3">
         <v>45102</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>45102</v>
       </c>
     </row>
@@ -588,6 +623,15 @@
       <c r="B7" s="3">
         <v>45116</v>
       </c>
+      <c r="C7" s="3">
+        <v>45126</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45126</v>
+      </c>
+      <c r="E7" s="4">
+        <v>45126</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -612,7 +656,7 @@
       <c r="D10" s="3">
         <v>45098</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>45098</v>
       </c>
     </row>
@@ -657,7 +701,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A1:XFD1048576"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -702,29 +746,22 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -733,7 +770,6 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -756,7 +792,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A1:XFD1048576"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -801,32 +837,27 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -835,7 +866,6 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -868,7 +898,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -903,39 +933,41 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="E6" s="4"/>
+      <c r="A6" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="B7" s="3"/>
-      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -959,13 +991,102 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF595FB-D905-4D1A-BB35-7BB95349353D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74.7109375" style="2" customWidth="1"/>
+    <col min="2" max="4" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -974,11 +1095,21 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
gvar code finished (but not tested)
</commit_message>
<xml_diff>
--- a/Design/Euphoria Rev1 Task List.xlsx
+++ b/Design/Euphoria Rev1 Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Euphoria\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30EA8ED-FA61-4EC3-968D-9A2DC5DFFCF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A45B4AB-37DC-4AEF-A4D4-FCEFF6521B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12435" yWindow="750" windowWidth="21615" windowHeight="11325" activeTab="3" xr2:uid="{283B4835-3097-4296-82F0-26B49D49393F}"/>
+    <workbookView xWindow="2355" yWindow="405" windowWidth="21615" windowHeight="11325" xr2:uid="{283B4835-3097-4296-82F0-26B49D49393F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tier 0" sheetId="1" r:id="rId1"/>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1EC2650-86F8-4191-84AB-CF07FD671912}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -641,6 +641,9 @@
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45138</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -897,7 +900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872012C2-CA93-45EE-9438-F46C4A342CBD}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>

</xml_diff>